<commit_message>
Update Excel file and add images of results
</commit_message>
<xml_diff>
--- a/design.xlsx
+++ b/design.xlsx
@@ -5,7 +5,6 @@
   <sheets>
     <sheet state="visible" name="Avocado" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="posit" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Heart" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -31,7 +30,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -86,18 +85,6 @@
         <bgColor rgb="FFE76534"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF352F2E"/>
-        <bgColor rgb="FF352F2E"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor theme="5"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -105,7 +92,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -117,8 +104,6 @@
     <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="10" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="11" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -143,10 +128,6 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1336,61 +1317,4 @@
   </conditionalFormatting>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="1" max="23" width="3.0"/>
-  </cols>
-  <sheetData>
-    <row r="2">
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-    </row>
-    <row r="3">
-      <c r="G3" s="9"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="9"/>
-    </row>
-    <row r="4">
-      <c r="G4" s="9"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="9"/>
-    </row>
-    <row r="5">
-      <c r="H5" s="9"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="9"/>
-    </row>
-    <row r="6">
-      <c r="I6" s="9"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="9"/>
-    </row>
-    <row r="7">
-      <c r="J7" s="9"/>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>